<commit_message>
Data up to episode 10 and cleaning up of solutions generator
</commit_message>
<xml_diff>
--- a/data/vip2024.xlsx
+++ b/data/vip2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelhaas/Documents/Coding/aytogermany/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEB22C7-A91E-E344-9DF0-5BFCBAA1941E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDCD6AA-F033-AF41-BD36-4F12CDEAC91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15500" yWindow="780" windowWidth="18600" windowHeight="18860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12820" yWindow="780" windowWidth="21280" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nights" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
   <si>
     <t>Alex</t>
   </si>
@@ -107,7 +107,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +117,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -163,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -181,6 +199,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,10 +508,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -544,13 +566,13 @@
       <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="8" t="s">
         <v>12</v>
       </c>
       <c r="H2" t="s">
@@ -570,16 +592,16 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
@@ -594,7 +616,7 @@
       <c r="I3" t="s">
         <v>13</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="8" t="s">
         <v>17</v>
       </c>
       <c r="K3" t="s">
@@ -602,6 +624,76 @@
       </c>
       <c r="L3" s="5">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data up to episode 16
</commit_message>
<xml_diff>
--- a/data/vip2024.xlsx
+++ b/data/vip2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelhaas/Documents/Coding/aytogermany/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDCD6AA-F033-AF41-BD36-4F12CDEAC91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3958A5FB-CB2E-974C-8A93-4BF4FF1322F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12820" yWindow="780" windowWidth="21280" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="780" windowWidth="33920" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nights" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="22">
   <si>
     <t>Alex</t>
   </si>
@@ -128,13 +128,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,8 +201,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,10 +508,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -557,10 +557,10 @@
       </c>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -569,22 +569,22 @@
       <c r="E2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="L2" s="5">
@@ -595,28 +595,28 @@
       <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>17</v>
       </c>
       <c r="K3" t="s">
@@ -627,7 +627,7 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -639,16 +639,16 @@
       <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" t="s">
         <v>19</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="7" t="s">
@@ -694,6 +694,111 @@
       </c>
       <c r="L5" s="5">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="5">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
json schema und daten cleanup
</commit_message>
<xml_diff>
--- a/data/vip2024.xlsx
+++ b/data/vip2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isabelhaas/Documents/Coding/aytogermany/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6167A03D-4B8F-F447-A18F-D4A3465DAF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C9F0E6-3678-0D43-8D13-7C12700FA526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13120" yWindow="780" windowWidth="20920" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="22">
   <si>
     <t>Alex</t>
   </si>
@@ -493,10 +493,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -821,6 +821,41 @@
         <v>7</v>
       </c>
     </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="5">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>